<commit_message>
Revised king devick I/O
</commit_message>
<xml_diff>
--- a/participants/participant_02/participant_02_conditions.xlsx
+++ b/participants/participant_02/participant_02_conditions.xlsx
@@ -9753,9 +9753,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8409419D26D7C4EB6DFA2C65A4F9BE1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e047ffe372120ce8cabd068ee4438d3d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="817b719d-a72b-49ed-9c44-b17aa9d4c465" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="204ca46f898a7194094cd90c07b0cb79" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8409419D26D7C4EB6DFA2C65A4F9BE1" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8e3c5ba4a77d7906c6e8ce7428cfdd58">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="817b719d-a72b-49ed-9c44-b17aa9d4c465" xmlns:ns3="2ce8a581-d4a9-432f-b0e2-c0b39f98f5b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="643c42d6e5ec6ef951078118cc7a2a3f" ns2:_="" ns3:_="">
     <xsd:import namespace="817b719d-a72b-49ed-9c44-b17aa9d4c465"/>
+    <xsd:import namespace="2ce8a581-d4a9-432f-b0e2-c0b39f98f5b2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -9766,6 +9767,8 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -9792,6 +9795,36 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2ce8a581-d4a9-432f-b0e2-c0b39f98f5b2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -9914,7 +9947,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B3E1E30-5F8A-431D-B9C8-2A59F89040CF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630849F-5B47-46F6-9575-E00FFDB7CD01}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>